<commit_message>
Validation Phase Result Added
</commit_message>
<xml_diff>
--- a/Data Analysis/Result.xlsx
+++ b/Data Analysis/Result.xlsx
@@ -101,13 +101,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +412,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,7 +427,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -442,23 +442,23 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -466,50 +466,140 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>0.64444195089672496</v>
+      </c>
+      <c r="C3">
+        <v>0.57679420009771498</v>
+      </c>
+      <c r="D3">
+        <v>1.2537402340823799E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>0.639741755592796</v>
+      </c>
+      <c r="C4">
+        <v>0.66737576791656394</v>
+      </c>
+      <c r="D4">
+        <v>1.26594542567377E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>0.64400234772562404</v>
+      </c>
+      <c r="C5">
+        <v>0.58001209282675303</v>
+      </c>
+      <c r="D5">
+        <v>1.25437175499044E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>0.75932645797729403</v>
+      </c>
+      <c r="C6">
+        <v>6.8614125000000001</v>
+      </c>
+      <c r="D6">
+        <v>4.8430510000000001E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>0.85400037812962104</v>
+      </c>
+      <c r="C7">
+        <v>0.428416795867057</v>
+      </c>
+      <c r="D7">
+        <v>7.2027827221347201E-4</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>0.79095507517726504</v>
+      </c>
+      <c r="C8">
+        <v>0.53355472755182398</v>
+      </c>
+      <c r="D8">
+        <v>9.3256825805548003E-4</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>0.90717716496461898</v>
+      </c>
+      <c r="C9">
+        <v>0.33961996526183902</v>
+      </c>
+      <c r="D9">
+        <v>4.7667283584392801E-4</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>0.96639268883587004</v>
+      </c>
+      <c r="C10">
+        <v>0.267330764018261</v>
+      </c>
+      <c r="D10">
+        <v>2.30317100128948E-4</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11">
+        <v>0.97038525885994098</v>
+      </c>
+      <c r="C11">
+        <v>0.28070083835049903</v>
+      </c>
+      <c r="D11">
+        <v>2.0328828731852101E-4</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0.80308792299610798</v>
+      </c>
+      <c r="C12">
+        <v>0.99511655463733995</v>
+      </c>
+      <c r="D12">
+        <v>8.3865796941974698E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Result Added as XLSX file
</commit_message>
<xml_diff>
--- a/Data Analysis/Result.xlsx
+++ b/Data Analysis/Result.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Result" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -87,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -95,19 +95,176 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +569,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,180 +583,270 @@
     <col min="7" max="7" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="B2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="16">
         <v>0.64444195089672496</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>0.57679420009771498</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="16">
         <v>1.2537402340823799E-3</v>
       </c>
+      <c r="E3" s="2">
+        <v>0.69287922677104996</v>
+      </c>
+      <c r="F3" s="16">
+        <v>6.0900221055888197</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.39963550074550203</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="8">
         <v>0.639741755592796</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>0.66737576791656394</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>1.26594542567377E-3</v>
       </c>
+      <c r="E4" s="2">
+        <v>0.69358180717974205</v>
+      </c>
+      <c r="F4" s="8">
+        <v>6.1759904411022202</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.39960608054272401</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="8">
         <v>0.64400234772562404</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>0.58001209282675303</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
         <v>1.25437175499044E-3</v>
       </c>
+      <c r="E5" s="2">
+        <v>0.69298910565721095</v>
+      </c>
+      <c r="F5" s="8">
+        <v>6.09430958762613</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.39964659061191399</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="8">
         <v>0.75932645797729403</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>6.8614125000000001</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="8">
         <v>4.8430510000000001E-3</v>
       </c>
+      <c r="E6" s="2">
+        <v>0.76403750975926699</v>
+      </c>
+      <c r="F6" s="8">
+        <v>12.483169999999999</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.39851530000000002</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="8">
         <v>0.85400037812962104</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>0.428416795867057</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <v>7.2027827221347201E-4</v>
       </c>
+      <c r="E7" s="2">
+        <v>0.74598290949312895</v>
+      </c>
+      <c r="F7" s="8">
+        <v>6.0606885493095897</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.40572546265339199</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="8">
         <v>0.79095507517726504</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>0.53355472755182398</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <v>9.3256825805548003E-4</v>
       </c>
+      <c r="E8" s="2">
+        <v>0.73033043248070895</v>
+      </c>
+      <c r="F8" s="8">
+        <v>6.0745297393575601</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.40417360668202401</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="8">
         <v>0.90717716496461898</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>0.33961996526183902</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>4.7667283584392801E-4</v>
       </c>
+      <c r="E9" s="2">
+        <v>0.76500275878601798</v>
+      </c>
+      <c r="F9" s="8">
+        <v>5.98866448207239</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.40340160308709899</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="8">
         <v>0.96639268883587004</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>0.267330764018261</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="8">
         <v>2.30317100128948E-4</v>
       </c>
+      <c r="E10" s="2">
+        <v>0.76738935917345497</v>
+      </c>
+      <c r="F10" s="8">
+        <v>6.0052543687156303</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.40376396711770202</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="8">
         <v>0.97038525885994098</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>0.28070083835049903</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="8">
         <v>2.0328828731852101E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="E11" s="2">
+        <v>0.76739432562267096</v>
+      </c>
+      <c r="F11">
+        <v>5.9821166542799098</v>
+      </c>
+      <c r="G11">
+        <v>0.403317279949158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="9">
         <v>0.80308792299610798</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>0.99511655463733995</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="9">
         <v>8.3865796941974698E-4</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.74492896128753106</v>
+      </c>
+      <c r="F12" s="9">
+        <v>6.5544678616571597</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.40319820979655702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>